<commit_message>
Bill.bpmn and Bill2.bpmn coding complete
</commit_message>
<xml_diff>
--- a/activity计划v1.xlsx
+++ b/activity计划v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github-program\springboot-activiti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9CA0728C-F6D3-4B09-B288-BA0C32B2568E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{315F0A0D-C416-4263-B72E-2BE2C939BEA5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23892" windowHeight="10356" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
   <si>
     <t>功能点</t>
   </si>
@@ -163,6 +163,10 @@
   </si>
   <si>
     <t>完整的流程流转联调及测试</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>秦森</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -688,7 +692,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -798,16 +802,19 @@
       <c r="A8" t="s">
         <v>31</v>
       </c>
-      <c r="C8" t="s">
-        <v>28</v>
+      <c r="C8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>32</v>
       </c>
-      <c r="C9" t="s">
-        <v>26</v>
+      <c r="C9" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
@@ -817,8 +824,11 @@
       <c r="A10" t="s">
         <v>33</v>
       </c>
-      <c r="C10" t="s">
-        <v>28</v>
+      <c r="C10" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -828,6 +838,9 @@
       <c r="C11" t="s">
         <v>26</v>
       </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -865,8 +878,8 @@
       <c r="A16" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C16" t="s">
-        <v>26</v>
+      <c r="C16" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>